<commit_message>
upd some phy, init ia
</commit_message>
<xml_diff>
--- a/latex/chemia/data.xlsx
+++ b/latex/chemia/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\latex\chemia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB0C95A-5783-4285-84A7-C8BB4AE5125E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397A6FB1-0379-4B95-973F-C555824511C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{FF8B44EF-0A4E-447B-B201-457A253A8939}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="17281" windowHeight="9983" xr2:uid="{FF8B44EF-0A4E-447B-B201-457A253A8939}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1471,8 +1471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D8895A-FF47-49ED-86AC-CFAE14CCB44C}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9"/>

</xml_diff>

<commit_message>
generally finishing chem ia, except for sec 2(hypoth & reasoning), sec 3.3 (graph) and sec 4.3 (sample processing)
</commit_message>
<xml_diff>
--- a/latex/chemia/data.xlsx
+++ b/latex/chemia/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\latex\chemia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397A6FB1-0379-4B95-973F-C555824511C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE691AD-8E54-474F-BDE4-AE521ABC18DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1837" yWindow="1837" windowWidth="17281" windowHeight="9983" xr2:uid="{FF8B44EF-0A4E-447B-B201-457A253A8939}"/>
+    <workbookView xWindow="-37" yWindow="8002" windowWidth="23235" windowHeight="13875" xr2:uid="{FF8B44EF-0A4E-447B-B201-457A253A8939}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Experiment</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -93,6 +93,46 @@
   </si>
   <si>
     <t>csquare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delta mass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delta volume</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pdeltaconc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deltac</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deltax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fullx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deltay</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fully</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -275,7 +315,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$16</c:f>
+              <c:f>Sheet1!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -329,7 +369,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$16</c:f>
+              <c:f>Sheet1!$L$2:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -533,6 +573,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -540,7 +581,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1135,16 +1175,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>345281</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>78582</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304982</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1649</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>383381</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>2382</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>343082</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104958</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1469,18 +1509,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D8895A-FF47-49ED-86AC-CFAE14CCB44C}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="8" max="8" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.75" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.25" customWidth="1"/>
+    <col min="15" max="15" width="17.5" customWidth="1"/>
+    <col min="16" max="16" width="16.125" customWidth="1"/>
+    <col min="17" max="17" width="13.875" customWidth="1"/>
+    <col min="18" max="18" width="12.875" customWidth="1"/>
+    <col min="19" max="19" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1491,25 +1538,55 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1520,28 +1597,66 @@
         <v>4.0919999999999996</v>
       </c>
       <c r="D2">
+        <v>1E-4</v>
+      </c>
+      <c r="E2">
         <v>100</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E13" si="0">C2/D2/0.2033</f>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G13" si="0">C2/E2/0.2033</f>
         <v>0.2012788981800295</v>
       </c>
-      <c r="F2">
+      <c r="H2">
+        <f>D2/C2+F2/E2</f>
+        <v>5.0244379276637345E-3</v>
+      </c>
+      <c r="I2">
+        <f>H2*G2</f>
+        <v>1.0113133300541073E-3</v>
+      </c>
+      <c r="J2">
         <v>4.2</v>
       </c>
-      <c r="G2">
+      <c r="K2">
         <v>1200</v>
       </c>
-      <c r="H2">
-        <f>F2*0.000041/G2</f>
+      <c r="L2">
+        <f>J2*0.000041/K2</f>
         <v>1.4350000000000001E-7</v>
       </c>
-      <c r="I2">
-        <f>F2*F2</f>
+      <c r="M2">
+        <f>J2*J2</f>
         <v>17.64</v>
       </c>
+      <c r="N2">
+        <f>AVERAGE(G2:G4)</f>
+        <v>0.19972618462042957</v>
+      </c>
+      <c r="O2">
+        <f>(MAX(G2:G4)-MIN(G2:G4))/2</f>
+        <v>1.5248401377274956E-3</v>
+      </c>
+      <c r="P2" t="str">
+        <f>_xlfn.CONCAT(TEXT(N2,"0.000"),"pm", TEXT(O2, "0.000"))</f>
+        <v>0.200pm0.002</v>
+      </c>
+      <c r="Q2">
+        <f>AVERAGE(L2:L4)</f>
+        <v>1.3666666666666667E-7</v>
+      </c>
+      <c r="R2">
+        <f>(MAX(L2:L4)-MIN(L2:L4))/2</f>
+        <v>5.1250000000000012E-9</v>
+      </c>
+      <c r="S2" t="str">
+        <f>_xlfn.CONCAT(TEXT(10000000*Q2,"0.000"), "\pm", TEXT(10000000*R2, "0.000"))</f>
+        <v>1.367\pm0.051</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:19">
       <c r="B3">
         <v>2</v>
       </c>
@@ -1549,28 +1664,42 @@
         <v>4.0593000000000004</v>
       </c>
       <c r="D3">
+        <v>1E-4</v>
+      </c>
+      <c r="E3">
         <v>100</v>
       </c>
-      <c r="E3">
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
         <f t="shared" si="0"/>
         <v>0.19967043777668472</v>
       </c>
-      <c r="F3">
+      <c r="H3">
+        <f t="shared" ref="H3:H16" si="1">D3/C3+F3/E3</f>
+        <v>5.0246347892493777E-3</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I16" si="2">H3*G3</f>
+        <v>1.0032710280373832E-3</v>
+      </c>
+      <c r="J3">
         <v>3.9</v>
       </c>
-      <c r="G3">
+      <c r="K3">
         <v>1200</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H16" si="1">F3*0.000041/G3</f>
+      <c r="L3">
+        <f>J3*0.000041/K3</f>
         <v>1.3325000000000001E-7</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I16" si="2">F3*F3</f>
+      <c r="M3">
+        <f t="shared" ref="M3:M16" si="3">J3*J3</f>
         <v>15.209999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:19">
       <c r="B4">
         <v>3</v>
       </c>
@@ -1578,28 +1707,42 @@
         <v>4.03</v>
       </c>
       <c r="D4">
+        <v>1E-4</v>
+      </c>
+      <c r="E4">
         <v>100</v>
       </c>
-      <c r="E4">
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>0.19822921790457451</v>
       </c>
-      <c r="F4">
-        <v>3.9</v>
-      </c>
-      <c r="G4">
-        <v>1200</v>
-      </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>1.3325000000000001E-7</v>
+        <v>5.0248138957816376E-3</v>
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
+        <v>9.9606492867683211E-4</v>
+      </c>
+      <c r="J4">
+        <v>3.9</v>
+      </c>
+      <c r="K4">
+        <v>1200</v>
+      </c>
+      <c r="L4">
+        <f>J4*0.000041/K4</f>
+        <v>1.3325000000000001E-7</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
         <v>15.209999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1610,28 +1753,66 @@
         <v>8.1372</v>
       </c>
       <c r="D5">
+        <v>1E-4</v>
+      </c>
+      <c r="E5">
         <v>100</v>
       </c>
-      <c r="E5">
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>0.40025577963600589</v>
       </c>
-      <c r="F5">
-        <v>6.9</v>
-      </c>
-      <c r="G5">
-        <v>1200</v>
-      </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>2.3575E-7</v>
+        <v>5.0122892395418573E-3</v>
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
+        <v>2.0061977373339894E-3</v>
+      </c>
+      <c r="J5">
+        <v>6.9</v>
+      </c>
+      <c r="K5">
+        <v>1200</v>
+      </c>
+      <c r="L5">
+        <f>J5*0.000041/K5</f>
+        <v>2.3575E-7</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
         <v>47.610000000000007</v>
       </c>
+      <c r="N5">
+        <f t="shared" ref="N3:N14" si="4">AVERAGE(G5:G7)</f>
+        <v>0.39941957697983277</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O3:O14" si="5">(MAX(G5:G7)-MIN(G5:G7))/2</f>
+        <v>8.3866207575014617E-4</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" ref="P3:P14" si="6">_xlfn.CONCAT(TEXT(N5,"0.000"),"pm", TEXT(O5, "0.000"))</f>
+        <v>0.399pm0.001</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q3:Q14" si="7">AVERAGE(L5:L7)</f>
+        <v>2.3916666666666667E-7</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R3:R14" si="8">(MAX(L5:L7)-MIN(L5:L7))/2</f>
+        <v>3.4166666666666542E-9</v>
+      </c>
+      <c r="S5" t="str">
+        <f t="shared" ref="S3:S14" si="9">_xlfn.CONCAT(TEXT(10000000*Q5,"0.000"), "\pm", TEXT(10000000*R5, "0.000"))</f>
+        <v>2.392\pm0.034</v>
+      </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:19">
       <c r="B6">
         <v>2</v>
       </c>
@@ -1639,28 +1820,42 @@
         <v>8.1030999999999995</v>
       </c>
       <c r="D6">
+        <v>1E-4</v>
+      </c>
+      <c r="E6">
         <v>100</v>
       </c>
-      <c r="E6">
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>0.3985784554845056</v>
       </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>1200</v>
-      </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>2.3916666666666667E-7</v>
+        <v>5.0123409559304465E-3</v>
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
+        <v>1.9978111165764876E-3</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>1200</v>
+      </c>
+      <c r="L6">
+        <f>J6*0.000041/K6</f>
+        <v>2.3916666666666667E-7</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:19">
       <c r="B7">
         <v>3</v>
       </c>
@@ -1668,28 +1863,42 @@
         <v>8.1203000000000003</v>
       </c>
       <c r="D7">
+        <v>1E-4</v>
+      </c>
+      <c r="E7">
         <v>100</v>
       </c>
-      <c r="E7">
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>0.3994244958189867</v>
       </c>
-      <c r="F7">
-        <v>7.1</v>
-      </c>
-      <c r="G7">
-        <v>1200</v>
-      </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>2.4258333333333331E-7</v>
+        <v>5.0123148159550756E-3</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
+        <v>2.0020413182488934E-3</v>
+      </c>
+      <c r="J7">
+        <v>7.1</v>
+      </c>
+      <c r="K7">
+        <v>1200</v>
+      </c>
+      <c r="L7">
+        <f>J7*0.000041/K7</f>
+        <v>2.4258333333333331E-7</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
         <v>50.41</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1700,28 +1909,66 @@
         <v>12.1982</v>
       </c>
       <c r="D8">
+        <v>1E-4</v>
+      </c>
+      <c r="E8">
         <v>100</v>
       </c>
-      <c r="E8">
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>0.60000983767830784</v>
       </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>1200</v>
-      </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>3.4166666666666664E-7</v>
+        <v>5.0081979308422555E-3</v>
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
+        <v>3.0049680275454991E-3</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>1200</v>
+      </c>
+      <c r="L8">
+        <f>J8*0.000041/K8</f>
+        <v>3.4166666666666664E-7</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>0.60081160846040327</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>2.0191834727004698E-3</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="6"/>
+        <v>0.601pm0.002</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="7"/>
+        <v>3.4052777777777781E-7</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="8"/>
+        <v>1.7083333333333205E-9</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="9"/>
+        <v>3.405\pm0.017</v>
+      </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:19">
       <c r="B9">
         <v>2</v>
       </c>
@@ -1729,28 +1976,42 @@
         <v>12.2637</v>
       </c>
       <c r="D9">
+        <v>1E-4</v>
+      </c>
+      <c r="E9">
         <v>100</v>
       </c>
-      <c r="E9">
+      <c r="F9">
+        <v>0.5</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
         <v>0.60323167732415151</v>
       </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="G9">
-        <v>1200</v>
-      </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>3.4166666666666664E-7</v>
+        <v>5.0081541459755215E-3</v>
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
+        <v>3.0210772257747175E-3</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>1200</v>
+      </c>
+      <c r="L9">
+        <f>J9*0.000041/K9</f>
+        <v>3.4166666666666664E-7</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:19">
       <c r="B10">
         <v>3</v>
       </c>
@@ -1758,28 +2019,42 @@
         <v>12.1816</v>
       </c>
       <c r="D10">
+        <v>1E-4</v>
+      </c>
+      <c r="E10">
         <v>100</v>
       </c>
-      <c r="E10">
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
         <v>0.59919331037875057</v>
       </c>
-      <c r="F10">
-        <v>9.9</v>
-      </c>
-      <c r="G10">
-        <v>1200</v>
-      </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>3.3825E-7</v>
+        <v>5.0082091022525775E-3</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
+        <v>3.0008853910477125E-3</v>
+      </c>
+      <c r="J10">
+        <v>9.9</v>
+      </c>
+      <c r="K10">
+        <v>1200</v>
+      </c>
+      <c r="L10">
+        <f>J10*0.000041/K10</f>
+        <v>3.3825E-7</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
         <v>98.01</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1790,28 +2065,66 @@
         <v>16.2455</v>
       </c>
       <c r="D11">
+        <v>1E-4</v>
+      </c>
+      <c r="E11">
         <v>100</v>
       </c>
-      <c r="E11">
+      <c r="F11">
+        <v>0.5</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
         <v>0.79909001475651742</v>
       </c>
-      <c r="F11">
-        <v>12.9</v>
-      </c>
-      <c r="G11">
-        <v>1200</v>
-      </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>4.4075000000000003E-7</v>
+        <v>5.0061555507679052E-3</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
+        <v>4.0003689129365473E-3</v>
+      </c>
+      <c r="J11">
+        <v>12.9</v>
+      </c>
+      <c r="K11">
+        <v>1200</v>
+      </c>
+      <c r="L11">
+        <f>J11*0.000041/K11</f>
+        <v>4.4075000000000003E-7</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
         <v>166.41</v>
       </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>0.79881619937694703</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="5"/>
+        <v>6.4190850959178203E-4</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="6"/>
+        <v>0.799pm0.001</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="7"/>
+        <v>4.4075000000000003E-7</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="8"/>
+        <v>3.4166666666666675E-9</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="9"/>
+        <v>4.408\pm0.034</v>
+      </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:19">
       <c r="B12">
         <v>2</v>
       </c>
@@ -1819,28 +2132,42 @@
         <v>16.2241</v>
       </c>
       <c r="D12">
+        <v>1E-4</v>
+      </c>
+      <c r="E12">
         <v>100</v>
       </c>
-      <c r="E12">
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
         <v>0.79803738317757</v>
       </c>
-      <c r="F12">
-        <v>12.8</v>
-      </c>
-      <c r="G12">
-        <v>1200</v>
-      </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>4.3733333333333338E-7</v>
+        <v>5.0061636700957221E-3</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
+        <v>3.99510575504181E-3</v>
+      </c>
+      <c r="J12">
+        <v>12.8</v>
+      </c>
+      <c r="K12">
+        <v>1200</v>
+      </c>
+      <c r="L12">
+        <f>J12*0.000041/K12</f>
+        <v>4.3733333333333338E-7</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
         <v>163.84000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:19">
       <c r="B13">
         <v>3</v>
       </c>
@@ -1848,28 +2175,42 @@
         <v>16.2502</v>
       </c>
       <c r="D13">
+        <v>1E-4</v>
+      </c>
+      <c r="E13">
         <v>100</v>
       </c>
-      <c r="E13">
+      <c r="F13">
+        <v>0.5</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="0"/>
         <v>0.79932120019675357</v>
       </c>
-      <c r="F13">
-        <v>13</v>
-      </c>
-      <c r="G13">
-        <v>1200</v>
-      </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>4.4416666666666672E-7</v>
+        <v>5.0061537704151338E-3</v>
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
+        <v>4.0015248401377278E-3</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="K13">
+        <v>1200</v>
+      </c>
+      <c r="L13">
+        <f>J13*0.000041/K13</f>
+        <v>4.4416666666666672E-7</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1880,28 +2221,66 @@
         <v>20.160699999999999</v>
       </c>
       <c r="D14">
+        <v>1E-4</v>
+      </c>
+      <c r="E14">
         <v>100</v>
       </c>
-      <c r="E14">
-        <f>C14/D14/0.2033</f>
+      <c r="F14">
+        <v>0.5</v>
+      </c>
+      <c r="G14">
+        <f>C14/E14/0.2033</f>
         <v>0.99167240531234613</v>
-      </c>
-      <c r="F14">
-        <v>14.1</v>
-      </c>
-      <c r="G14">
-        <v>1200</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>4.8174999999999998E-7</v>
+        <v>5.0049601452330523E-3</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
+        <v>4.9632808657156906E-3</v>
+      </c>
+      <c r="J14">
+        <v>14.1</v>
+      </c>
+      <c r="K14">
+        <v>1200</v>
+      </c>
+      <c r="L14">
+        <f>J14*0.000041/K14</f>
+        <v>4.8174999999999998E-7</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
         <v>198.81</v>
       </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>0.99632234792588947</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="5"/>
+        <v>3.5169699950812205E-3</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="6"/>
+        <v>0.996pm0.004</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="7"/>
+        <v>4.9313888888888889E-7</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="8"/>
+        <v>1.366666666666667E-8</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="9"/>
+        <v>4.931\pm0.137</v>
+      </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:19">
       <c r="B15">
         <v>2</v>
       </c>
@@ -1909,28 +2288,42 @@
         <v>20.303699999999999</v>
       </c>
       <c r="D15">
+        <v>1E-4</v>
+      </c>
+      <c r="E15">
         <v>100</v>
       </c>
-      <c r="E15">
-        <f t="shared" ref="E15:E16" si="3">C15/D15/0.2033</f>
+      <c r="F15">
+        <v>0.5</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15:G16" si="10">C15/E15/0.2033</f>
         <v>0.99870634530250857</v>
-      </c>
-      <c r="F15">
-        <v>14.9</v>
-      </c>
-      <c r="G15">
-        <v>1200</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
-        <v>5.0908333333333332E-7</v>
+        <v>5.0049252106758868E-3</v>
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
+        <v>4.998450565666503E-3</v>
+      </c>
+      <c r="J15">
+        <v>14.9</v>
+      </c>
+      <c r="K15">
+        <v>1200</v>
+      </c>
+      <c r="L15">
+        <f>J15*0.000041/K15</f>
+        <v>5.0908333333333332E-7</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
         <v>222.01000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:19">
       <c r="B16">
         <v>3</v>
       </c>
@@ -1938,57 +2331,71 @@
         <v>20.301300000000001</v>
       </c>
       <c r="D16">
+        <v>1E-4</v>
+      </c>
+      <c r="E16">
         <v>100</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="3"/>
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="10"/>
         <v>0.9985882931628135</v>
-      </c>
-      <c r="F16">
-        <v>14.3</v>
-      </c>
-      <c r="G16">
-        <v>1200</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
-        <v>4.8858333333333337E-7</v>
+        <v>5.0049257929295167E-3</v>
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
+        <v>4.9978603049680272E-3</v>
+      </c>
+      <c r="J16">
+        <v>14.3</v>
+      </c>
+      <c r="K16">
+        <v>1200</v>
+      </c>
+      <c r="L16">
+        <f>J16*0.000041/K16</f>
+        <v>4.8858333333333337E-7</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
         <v>204.49</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
-      <c r="I18" t="s">
+    <row r="18" spans="1:15">
+      <c r="M18" t="s">
         <v>8</v>
       </c>
-      <c r="J18" t="s">
+      <c r="N18" t="s">
         <v>9</v>
       </c>
-      <c r="K18" t="s">
+      <c r="O18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="I19" t="s">
+    <row r="19" spans="1:15">
+      <c r="M19" t="s">
         <v>13</v>
       </c>
-      <c r="J19" t="s">
+      <c r="N19" t="s">
         <v>10</v>
       </c>
-      <c r="K19" t="s">
+      <c r="O19" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>